<commit_message>
Adjusted wetland trend data in CP and HAB to reflect the 2005 to 2010 NOAA CCAP change in coastal wetland extent. Trend based on most recent 5 years of data.
</commit_message>
<xml_diff>
--- a/prep/HAB/wetlands_trend.xlsx
+++ b/prep/HAB/wetlands_trend.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eschemmel/Documents/github/mhi/prep/HAB/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1200" windowWidth="20115" windowHeight="3540"/>
+    <workbookView xWindow="-32780" yWindow="580" windowWidth="24860" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wetlands_trend" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -49,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -581,6 +586,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -628,7 +636,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -661,9 +669,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -696,6 +721,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -871,16 +913,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="J13" sqref="J13:J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -909,7 +951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1992</v>
       </c>
@@ -952,7 +994,7 @@
         <v>-5.1483385946971376E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1992</v>
       </c>
@@ -975,11 +1017,11 @@
         <v>5.0640077999999998E-2</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:M6" si="0">C11-C3</f>
+        <f t="shared" ref="L3:L5" si="0">C11-C3</f>
         <v>0.91152139999999982</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M6" si="1">L3/C3</f>
+        <f t="shared" ref="M3:M5" si="1">L3/C3</f>
         <v>8.3159664632199301E-2</v>
       </c>
       <c r="N3">
@@ -987,7 +1029,7 @@
         <v>4.6199813684555165E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1992</v>
       </c>
@@ -1022,7 +1064,7 @@
         <v>-1.8134913660139862E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1992</v>
       </c>
@@ -1057,7 +1099,7 @@
         <v>-4.6561904914735625E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2005</v>
       </c>
@@ -1071,7 +1113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2005</v>
       </c>
@@ -1085,7 +1127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2005</v>
       </c>
@@ -1099,7 +1141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2005</v>
       </c>
@@ -1113,7 +1155,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2010</v>
       </c>
@@ -1130,7 +1172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2010</v>
       </c>
@@ -1144,7 +1186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2010</v>
       </c>
@@ -1158,7 +1200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2010</v>
       </c>
@@ -1170,6 +1212,44 @@
       </c>
       <c r="D13" t="s">
         <v>5</v>
+      </c>
+      <c r="I13">
+        <f>1-(C10/C6)</f>
+        <v>0.92745428323756873</v>
+      </c>
+      <c r="J13">
+        <f>-I13/5</f>
+        <v>-0.18549085664751375</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <f t="shared" ref="I14:I16" si="3">1-(C11/C7)</f>
+        <v>-0.48541454809328388</v>
+      </c>
+      <c r="J14">
+        <f>-I14/5</f>
+        <v>9.7082909618656774E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>0.29677150066468327</v>
+      </c>
+      <c r="J15">
+        <f>-I15/5</f>
+        <v>-5.9354300132936653E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>-0.11883871887522757</v>
+      </c>
+      <c r="J16">
+        <f>-I16/5</f>
+        <v>2.3767743775045515E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>